<commit_message>
full version of programme (draft)
</commit_message>
<xml_diff>
--- a/programme/Maths Psych_V2.xlsx
+++ b/programme/Maths Psych_V2.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amason/Documents/AMPC18/programme/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonfarrell/Simon/Admin/Conferences/AMPC18/website/programme/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="40180" windowHeight="24400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5800" yWindow="1120" windowWidth="40240" windowHeight="25720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Abstracts" sheetId="5" r:id="rId1"/>
@@ -73,10 +73,6 @@
     <t>Zhou</t>
   </si>
   <si>
-    <t xml:space="preserve">Source memory is memory for the context in which items were previously encountered. Past research has largely aimed to establish whether source memory retrieval is better characterised as a threshold or continuous process in two-alternative forced choice tasks, using ROC functions. Recently, Harlow and Donaldson (2013) introduced a continuous report paradigm to study performance in source memory tasks, and found evidence of a retrieval threshold underlying response accuracy. However, this account does not consider response time (RT) distributions. To investigate the role of decision-making in source memory retrieval, this study used the Smith (2016) circular diffusion model to introduce diffusion analogues of the threshold and continuous models of source memory retrieval in a replication of the Harlow and Donaldson (2013) task. Model selection done using the BIC found support for a circular diffusion model where memory discretely fails, as both RT and response accuracy data suggested that there were two components in performance. 
-</t>
-  </si>
-  <si>
     <t>Oberauer</t>
   </si>
   <si>
@@ -293,22 +289,12 @@
     <t>University of Queensland</t>
   </si>
   <si>
-    <t xml:space="preserve">Whilst much is known about the effects of rewards and punishments on motivation and behavior, far less is known about their effects on the underlying information processing structures. A view held by many is that the human information processing system has a limited capacity. The system must therefore manage its resources efficiently, taking into account the supply of and demand for resources when deploying them to various tasks. According to this perspective, reward and punishment might increase the rate of information processing, because it makes the allocation of resources to a task a more worthwhile investment. An alternative perspective is that the potential for reward or punishment may slow the processing of information, because they increase the need for resources to be deployed toward off-task activities such as self-monitoring. 
-We examined these predictions using a random dot motion detection task in which participants viewed clouds of moving dots and had to determine whether the dots were moving mostly left or mostly right. For each block, the participants were given the goal of being more accurate and faster than the average participant in a pilot study. In the reward condition, participants gained money for achieving the goal. In the punishment condition, participants lost money for failing the goal. The rate of information processing was measured by estimating the drift rate parameter using the LBA model within a hierarchical Bayesian framework.
-When participants were given an opportunity for reward, the average rate of information processing did not change from baseline. However, the amount of information required to make a decision (i.e., response threshold) increased. When participants were under threat of punishment, the average rate of information processing decreased, and the amount of information required to make a decision also decreased. These findings demonstrate the need to consider the context when attempting to understand how information processing will unfold.
-</t>
-  </si>
-  <si>
     <t>Human information processing in the face of reward versus punishment</t>
   </si>
   <si>
     <t>Little</t>
   </si>
   <si>
-    <t xml:space="preserve">We propose an adaptation of the logical rule-based models (Fific, Little &amp; Nosofsky, 2010) in order to characterise decision making based on information held in visual short term memory. Specifically, we seek to diagnose decision making processes in a one-shot multi-element change detection task, as either serial, parallel, or coactive in nature. We additionally seek to characterise whether the integration rule for each change decision is based on the maximum evidence strength or the sum of strengths across elements. The logical rule models assume that each element is represented as a Gaussian distribution of perceptual effects. To model changes, we assume that the strength of the change is represented as a folded-normal distribution.  We factorially manipulate the magnitude of change for a given element and whether a change decision requires an OR or an AND decision rule. This approach is novel in that it provides a way to unify signal detection models of change detection (Maximum Difference and Summed Difference models) with models of information process.
- </t>
-  </si>
-  <si>
     <t>Stephens</t>
   </si>
   <si>
@@ -366,32 +352,18 @@
     <t>Thompson</t>
   </si>
   <si>
-    <t xml:space="preserve">What forensic experts should say, or should be allowed to say, about the results of forensic comparisons has been a contentious issue in the legal and forensic science communities. It is common practice for forensic pattern identification experts, such as in fingerprints and ballistics, to testify that two impressions originate from the same source to the exclusion of all others in the absence of statistical information. Experts have even claimed 100% accuracy, or that the rates of error are so improbable that they need not be considered. An alternative framework is necessary. When, if ever, should experts claim to have determined that two items share a common source, and should they present error rates, or the probability of coincidental matches?
-Here we explore options for the statistical representation and communication of forensic evidence in court. We argue that we have reached a turning point, where Australian state and federal police jurisdictions are seeking alternative frameworks for presenting evidence in court, but where well-considered proposals are scarce. We propose an avenue by which the mathematical psychology community might lend their own expertise to the problem.
-</t>
-  </si>
-  <si>
     <t>Dennis</t>
   </si>
   <si>
     <t>Predicting memory for WHEN</t>
   </si>
   <si>
-    <t xml:space="preserve">We present a model that predicts when people will believe events from their lives occurred on a person by person and stimulus by stimulus basis. Participants wore a smartphone in a pouch around their necks for two weeks. The smartphone collected timestamps, GPS, accelerometry, audio segments and images. These data sources were augmented with weather conditions, temperature, moon phase and tags derived from the audio using a machine learning model. A week later they were shown a selection of images and were required to indicate on which day each was taken. A conditional logit model predicted leave one person out judgements, leave one day out judgements and leave one observation out judgements. We highlight the advantages of using cross validation over other methods of model selection.
-</t>
-  </si>
-  <si>
     <t>1University of Melbourne, 2University of Newcastle, 3Vanderbilt University, 4NIH Research Laboratories</t>
   </si>
   <si>
     <t>Extensional and intensional reasoning: A Bayesian perspective on the conjunction fallacy</t>
   </si>
   <si>
-    <t>The conjunction fallacy is one of the most striking findings in the heuristics and biases literature, in which people rate a pair of propositions (e.g. Linda is a bank teller and a feminist) as more probable than one of the constituents (e.g. Linda is a bank teller). This is especially likely to occur when the description of Linda is more representative of one category (feminist) than the other. An extensive literature on the conjunction fallacy demonstrates that the effect is robust, but also sensitive to linguistic and pragmatic factors. 
-In this talk we present a Bayesian perspective on the problem. Extending earlier work on the pragmatics of conjunction effects, we argue that there is a degree of ambiguity to the inference problem that people need to solve. In an extensional reasoning scenario the problem is assumed to be to infer the properties that Linda has (in the world) and it cannot be the case that Linda is a feminist bank teller without also being a bank teller. In an intensional reasoning scenario the goal is to identify the meaning of the ideas being described or communicated. Intensional reasoning allows a conjunction to be more likely than a constituent: if my intent is to communicate “red circle” to you, and you infer “circle”, a communication failure has occurred. In an effective communicative system, it is necessary to be able to specify (and to infer) the smaller of two nested sets, and conjunction 'fallacies’ are necessarily permitted. Consequently, while probabilistic reasoning models based on extensional logic do not produce conjunction fallacies, it is entirely possible for an intensional reasoning system to do so. 
-Motivated by this theoretical perspective we present a series of experiments showing that people's behaviour in these tasks is highly sensitive to the distinction between extensional and intensional semantics. When a reasoning problem is framed in a way that emphasises the communicative and social aspect to the situation, strong conjunction effects appear. When the task is reframed to emphasise the extensional and non-social aspects, the fallacy is either attenuated or absent. This sensitivity occurs across many different social categories (e.g. feminist bank tellers) as well as reasoning about purely physical events (dice rolls). We argue that this sensitivity to framing occurs because people switch between solving different inference problems, both of which are sensible but are not equivalent to each other.</t>
-  </si>
-  <si>
     <t>Navarro</t>
   </si>
   <si>
@@ -408,12 +380,6 @@
   </si>
   <si>
     <t>Near neighbour judgements as an efficient way to estimate semantic similarity.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A popular way to estimate how words are similar involves asking participants to assign a magnitude judgement of similarity for a pair of words using a rating scale. This method has various limitations associated with the use of rating scales and lack of context when only two items are compared. Moreover, from a practical point of view, the procedure becomes prohibitively expensive for a large number of items. For example, for 1,000 items, obtaining one observation per pair would require nearly half a million judgements.
-In two studies, we explore an alternative procedure in which  participants either generate or rank a small number of near neighbours to a natural language concept. To evaluate the validity of this new task, we used pair-wise similarities collected for 15 basic level categories such as “birds” or “tools”. For each of the categories, we construct a sparse near neighbour graph and show that a mechanism of spreading activation based on random walks (see De Deyne, Navarro, Perfors &amp; Storms, 2016) can be used to accurately predict pair-wise similarity judgements using a limited amount of information.
-While these results suggest excellent external validity at a fraction of the cost, we also discuss some theoretical implications about the number of near neighbours and fundamental differences between similarity-based and feature-based inference in natural language concepts.
-</t>
   </si>
   <si>
     <t>Lo</t>
@@ -608,11 +574,6 @@
     <t>Most psychological theories of cognition propose that when an individual encounters a task, they rely on a mental representation of the stimuli used in that task. Standard approaches for measuring the mental representation of such stimuli are explicit and subjective. For example, observers may be asked to rate what they believe to be the similarity between pairs of items. One of the major issues with this approach is that one must assume that the stimuli have the same mental representation in the similarity rating task as in any other task. Our approach is to subvert this problem, by directly extracting the mental representation of stimuli from the cognitive task of interest. Specifically, we use the Generalized Context Model to infer the mental representation of a set of 20 colors from responses in a visual working memory task. Along the way, we also use the model to infer the strength of memories for items on the current and previous trial, thus investigating the role of recency, primacy, and proactive interference in visual working memory. Finally, we also use the model to infer the mental representation of 20 letter stimuli in a verbal working memory task.</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Throughout the last few decades, a heated debate has been going on between frequentists and Bayesians. There are substantial theoretical and philosophical differences between both methods. Recently, a number of papers have come out claiming that for pragmatic purposes, both philosophies may not be all that different. In this presentation, I will discuss work that examines numerical correspondence between frequentist confidence intervals and Bayesian credible intervals based on non-informative priors. I show that numerically the differences between confidence intervals and credible intervals are very often negligible. I'll conclude with my take on the consequences of this for the frequentist-Bayesian debate from a practical viewpoint.
-</t>
-  </si>
-  <si>
     <t>Credible Confidence: A pragmatic view on the frequentist vs Bayesian debate</t>
   </si>
   <si>
@@ -629,10 +590,6 @@
   </si>
   <si>
     <t>Memory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I present a model for decision making for stimuli and responses in continuous space.  The model is applied to three numeracy tasks: in one, a two-digit number is presented and the participant has to move their finger to a matching location on a number line, in the second, an array of dots is presented and the participant is to move their finger to a matching location on an arc, and in the third, an array of dots is presented and the participant has to speak the number.  The model is composed of diffusion processes on lines and planes in which evidence from a stimulus (distributed across space) drives the noisy decision process which accumulates evidence over time to a criterion at which point a response is initiated.  Noise is represented as a continuous Gaussian process. The model produces fits for the full distributions of response times and choice probabilities across the stimulus space and
-</t>
   </si>
   <si>
     <t>Campitelli</t>
@@ -1066,10 +1023,6 @@
     <t>Syracuse University</t>
   </si>
   <si>
-    <t xml:space="preserve">
-Output interference is the finding that performance declines with test trial.  In cued recall tasks, participants are presented with a cue word and tasked to output the target word studied alongside.    Participants may choose to respond or not, and a response if given may be correct or incorrect.  We aim to understand the empirical pattern of output interference in cued recall and the underlying theoretical mechanisms.  We first analyzed published cued recall data and found fewer correct and incorrect responses across test trial.  Next, we tested the contribution of cue and target memories on output interference through a release from output interference paradigm: one member of each pair was an exemplar from one of two categories, and that member was either the cue word or target word (post-cued).  The critical comparison was when one category was tested in a blocked fashion and the blocking was either by cue category or by target category. We found that release from output interference only occurred when the test probe included information about the blocked words.  Specifically, release occurred for blocked cues; release occurred for blocked targets only when the test probe included the target category, in effect treating the target category like an extra cue. Together these data suggest that interference is driven both by learning the test probe and by imperfect filtering of already provided responses.  </t>
-  </si>
-  <si>
     <t>**Don van Ravenzwaai**, Casper Albers, Henk Kiers</t>
   </si>
   <si>
@@ -1176,10 +1129,6 @@
   </si>
   <si>
     <t>Christina Van Heer [1], Robert Hester [1], David K. Sewell [2], &amp; Philip L. Smith [1]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matthew B. Thompson [1], Rachel A. Searston [2], Gianni Ribeiro [3], &amp; Jason M. Tangen [3]
-</t>
   </si>
   <si>
     <t>Luke Strickland [1], David Elliott [1], Michael David Wilson [2], Shayne Loft [2], &amp; Andrew Heathcote [1]</t>
@@ -1593,11 +1542,6 @@
   </si>
   <si>
     <t>*University of Western Australia*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-*The Chinese University of Hong Kong*
-</t>
   </si>
   <si>
     <t>*University of Basel*</t>
@@ -1858,10 +1802,6 @@
     <t>**HOW DO PEOPLE THINK ABOUT THE PROBABILITY OF HUMAN EXTINCTION?**</t>
   </si>
   <si>
-    <t xml:space="preserve">**MODELLING SPEEDED MULTIELEMENT DECISION MAKING AS DIFFUSION IN A HYPERSPHERE**
-</t>
-  </si>
-  <si>
     <t>**ASSESSING ROBUSTNESS OF STATISTICAL MODELS: INFO-GAP THEORY**</t>
   </si>
   <si>
@@ -1871,10 +1811,6 @@
     <t>**MODELLING PROSPECTIVE MEMORY IN SIMULATED MARITIME SURVEILLANCE: COGNITIVE CONTROL AND COMPETITION FOR CAPACITY**</t>
   </si>
   <si>
-    <t xml:space="preserve">**ALTERNATIVE STATISTICAL FRAMEWORKS FOR COMMUNICATING THE STRENGTH OF FORENSIC EVIDENCE IN COURT**
-</t>
-  </si>
-  <si>
     <t>**THE ROLE OF PREDICTION ERROR AND CONFIDENCE IN SEQUENTIAL DECISIONS **</t>
   </si>
   <si>
@@ -1896,27 +1832,9 @@
     <t>**USING RESPONSE TIMES TO DISTINGUISH BETWEEN ATTRIBUTE-WISE AND ALTERNATE-WISE MODELS OF INTER-TEMPORAL CHOICE.**</t>
   </si>
   <si>
-    <t xml:space="preserve">In the real world we are often faced with decisions in which the possible outcomes are extremely good or bad but the probability of that outcome is extremely low: winning the lottery or being struck by lightning are prototypical examples. Should you buy a lottery ticket? Should you climb to the top of a hill in a rainstorm? These kind of situations are known colloquially as &amp;#39;Black Swan&amp;#39; scenarios and create a particularly hard decision problem. However, despite decades of research, decision theory is relatively silent about how people do (or should) reason about them: most of the standard tasks involve probabilities ranging between 10&amp;#37; to 90 &amp;#37; and the outcomes are a manageable fraction of existing savings. In this study we evaluate how people reason in situations when one or both options involve extremely low probabilities (from 0.1 to 1.5 &amp;#37;) of very bad outcomes (losing all of the points accumulated so far). We explore how decisions change as a function of the number of points available and the number of &amp;#39;black swan&amp;#39; options available. In addition, we evaluate if people's approach varies based on whether they are making a single bet or planning a strategy of bets over multiple games. Finally, we present some exploratory research investigating whether individual differences in anxiety and tolerance of uncertainty predict differences in behaviour in black swan situations. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">We generalize the circular 2D diffusion model of Smith (2016) to provide a new model of speeded decision-making in multielement visual displays. We model decision making in tasks with multielement displays as evidence accumulation by a vector-valued diffusion process in a hypersphere, whose radius represents the decision criterion for the task. We show that the methods used to derive response time and accuracy predictions for the 2D model can be applied, with only minor changes, to predict performance in higher dimensional spaces as well. We apply the model to the double-target deficit paradigm of Duncan (1980) in which participants judge whether briefly-presented four-element displays contain one or two digit targets among letter distractors. A 4D version of the hyperspherical diffusion model correctly predicted distributions of response times and response accuracy as a function of task difficulty in single-target and double-target versions of the task. The estimated drift rate parameters from the model imply that the mental representation of the decision alternatives, which we term the &amp;#39;decision template&amp;#39; for the task, encodes both configural and local stimulus properties. Along with its application to multielement decision making, the model has the potential to characterize the speed and accuracy of multiattribute decisions in studies of cognitive categorization, visual attention, and other areas.
-</t>
-  </si>
-  <si>
     <t>Amy Perfors &amp; Nicholas van Dam</t>
   </si>
   <si>
-    <t xml:space="preserve">Decisions from experience often differ from decisions based on described alternatives. This may stem from the fact that decisions from experience require that individuals learn about their choice alternatives by observing potential outcomes. We investigated the roles of attention and memory in the choice process by comparing two types of decision procedures: a) one where monetary value information is present during sampling, and b) one where values are revealed after sampling. In three experiments participants made a series of choices between pairs of risky gambles represented as urns containing different mixtures of blue and red balls. They began each trial by sampling balls from each urn. After observing a representative sample from each urn, participants chose which urn they would like to draw from for a consequential payment. In Experiment 3 some outcome samples were highlighted to increase visual and auditory salience.
-Results from all three experiments suggest that individuals place greater weight on rare events when outcome values are absent during sampling. This pattern is roughly consistent with the ‘description-experience gap’, in which decisions from description – which likewise involve separable representations of value and probability information – also indicate greater weighting of rare events relative to decisions from experience – which do not. In Experiment 3, we found that highlighting a rare reward increased its salience when outcome values were present, but not when they were absent, suggesting that highlighting rare outcome values during sampling led participants to place greater weight on these outcomes when making their choices. Parameter estimates from a hierarchical Bayesian prospect theory model supported the conclusion that value-absent choices involved greater overweighting of rare events. We discuss the implications of these findings on our understanding of the interplay between attention, memory, and choice. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This project uses Bayesian Linear Ballistic Accumulator (LBA) models of decision-making to model the cognitive control mechanisms that aid prospective memory (PM) and ongoing task performance in a complex and dynamic air-traffic control (ATC) simulation. We aim to explain how operators balance competing demands from ongoing and PM tasks under different levels of time pressure, task load, and relative response importance.
-The ATC task involved classifying pairs of moving aircraft as either 'in-conflict' or 'not in-conflict'. On some trials aircraft also contained a PM target which required execution of an atypical PM response. These decisions require the integration of multiple information sources (e.g., relative distance, airspeed) on a dynamic display while balancing several competing task requirements (e.g., time pressure, PM demands, relative response importance). Moreover, decisions typically unfolded over relatively long time-scales (up to 10 seconds). Initial work suggests that models of simple choice such as the LBA can account for ongoing and PM task performance in these complex, long time-scale, less controlled applied settings. 
-Our modelling shows evidence of both proactive and reactive control mechanisms. In terms of proactive control, response thresholds were higher under PM load. This suggests individuals proactively raise ongoing task thresholds when holding PM intentions. This effect was larger when the importance of the PM task was emphasised and smaller when the importance of the ongoing task was emphasised. This suggests that holding PM intentions encourages operators to make deliberate strategic adjustments to how they perform their primary ongoing task, and that these adjustments vary systematically as a function of PM task importance. 
-</t>
-  </si>
-  <si>
     <t>Mullard</t>
   </si>
   <si>
@@ -1933,13 +1851,6 @@
   </si>
   <si>
     <t>**CHARACTERISING THE ARCHITECTURE AND INTEGRATION OF CHANGE DETECTION DECISIONS**</t>
-  </si>
-  <si>
-    <t>Risky choice involves selection between two or more options each of which is a set of *n* ordered pairs, (*p&lt;sub&gt;i,x&lt;sub&gt;i*) , where *xi* is a (positive, negative, or zero) payoff and *pi* is its probability of occurrence, with  .  There are a large number of different models of risky choice that fall into two broad classes; fixed utility models that satisfy the condition of *simple scalability* and everything else. A prominent example of the former is Cumulative Prospect Theory (Tversky &amp; Kahneman, 1992); a prominent example of the latter is Decision Field Theory (Busemeyer &amp; Townsend, 1993). While it is known that behaviour can be observed that inconsistent with all models, this has largely been based on the construction of special cases. We decided to test the class of fixed utility models against a set of relatively unselected risky choices using signed difference analysis (SDA). The advantage of this approach is that there is no requirement to posit a particular form for the error function that links the difference in the utility of two gambles, *A* and *B*, with the probability of choosing *A* over *B*, *P(A&gt;B)* . We presented groups of participants with 30 *variable* gambles (*A*) each paired with one of four *fixed* gambles (*B*) and tested the prediction of fixed utility models that *P(A&gt;B)* has the same order over *A* for all *B* using the statistical test developed by Kalish, Dunn, Burdakov and Sysoev (2016). We discuss the implications of the results and explore a relatively simple extension to a (minimally) more complex model.
-*References* 
-Busemeyer, J. R., &amp; Townsend, J. T. (1993) Decision Field Theory: A dynamic cognition approach to decision making. *Psychological Review, 100*, 432–459.
-Kalish, M. L., Dunn, J. C., Burdakov, O. P., &amp; Sysoev, O. (2016). A statistical test for equality of latent orders. *Journal of Mathematical Psychology, 70*, 1-11
-Tversky, A. &amp; Kahneman, D. (1992). Advances in prospect theory: Cumulative representation of uncertainty. *Journal of Risk and Uncertainty, 5(4)*, 297–323.</t>
   </si>
   <si>
     <r>
@@ -1955,6 +1866,63 @@
       </rPr>
       <t xml:space="preserve">Our findings indicate that when participants complete both memory and evaluation tasks there is a cost to memory accuracy, but memory is still an effective strategy for performing evaluation. </t>
     </r>
+  </si>
+  <si>
+    <t>Matthew B. Thompson [1], Rachel A. Searston [2], Gianni Ribeiro [3], &amp; Jason M. Tangen [3]</t>
+  </si>
+  <si>
+    <t>*The Chinese University of Hong Kong*</t>
+  </si>
+  <si>
+    <t>Whilst much is known about the effects of rewards and punishments on motivation and behavior, far less is known about their effects on the underlying information processing structures. A view held by many is that the human information processing system has a limited capacity. The system must therefore manage its resources efficiently, taking into account the supply of and demand for resources when deploying them to various tasks. According to this perspective, reward and punishment might increase the rate of information processing, because it makes the allocation of resources to a task a more worthwhile investment. An alternative perspective is that the potential for reward or punishment may slow the processing of information, because they increase the need for resources to be deployed toward off-task activities such as self-monitoring.\\We examined these predictions using a random dot motion detection task in which participants viewed clouds of moving dots and had to determine whether the dots were moving mostly left or mostly right. For each block, the participants were given the goal of being more accurate and faster than the average participant in a pilot study. In the reward condition, participants gained money for achieving the goal. In the punishment condition, participants lost money for failing the goal. The rate of information processing was measured by estimating the drift rate parameter using the LBA model within a hierarchical Bayesian framework.\\When participants were given an opportunity for reward, the average rate of information processing did not change from baseline. However, the amount of information required to make a decision (i.e., response threshold) increased. When participants were under threat of punishment, the average rate of information processing decreased, and the amount of information required to make a decision also decreased. These findings demonstrate the need to consider the context when attempting to understand how information processing will unfold.</t>
+  </si>
+  <si>
+    <t>We propose an adaptation of the logical rule-based models (Fific, Little &amp; Nosofsky, 2010) in order to characterise decision making based on information held in visual short term memory. Specifically, we seek to diagnose decision making processes in a one-shot multi-element change detection task, as either serial, parallel, or coactive in nature. We additionally seek to characterise whether the integration rule for each change decision is based on the maximum evidence strength or the sum of strengths across elements. The logical rule models assume that each element is represented as a Gaussian distribution of perceptual effects. To model changes, we assume that the strength of the change is represented as a folded-normal distribution.  We factorially manipulate the magnitude of change for a given element and whether a change decision requires an OR or an AND decision rule. This approach is novel in that it provides a way to unify signal detection models of change detection (Maximum Difference and Summed Difference models) with models of information process.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output interference is the finding that performance declines with test trial.  In cued recall tasks, participants are presented with a cue word and tasked to output the target word studied alongside.    Participants may choose to respond or not, and a response if given may be correct or incorrect.  We aim to understand the empirical pattern of output interference in cued recall and the underlying theoretical mechanisms.  We first analyzed published cued recall data and found fewer correct and incorrect responses across test trial.  Next, we tested the contribution of cue and target memories on output interference through a release from output interference paradigm: one member of each pair was an exemplar from one of two categories, and that member was either the cue word or target word (post-cued).  The critical comparison was when one category was tested in a blocked fashion and the blocking was either by cue category or by target category. We found that release from output interference only occurred when the test probe included information about the blocked words.  Specifically, release occurred for blocked cues; release occurred for blocked targets only when the test probe included the target category, in effect treating the target category like an extra cue. Together these data suggest that interference is driven both by learning the test probe and by imperfect filtering of already provided responses.  </t>
+  </si>
+  <si>
+    <t>The conjunction fallacy is one of the most striking findings in the heuristics and biases literature, in which people rate a pair of propositions (e.g. Linda is a bank teller and a feminist) as more probable than one of the constituents (e.g. Linda is a bank teller). This is especially likely to occur when the description of Linda is more representative of one category (feminist) than the other. An extensive literature on the conjunction fallacy demonstrates that the effect is robust, but also sensitive to linguistic and pragmatic factors.\\In this talk we present a Bayesian perspective on the problem. Extending earlier work on the pragmatics of conjunction effects, we argue that there is a degree of ambiguity to the inference problem that people need to solve. In an extensional reasoning scenario the problem is assumed to be to infer the properties that Linda has (in the world) and it cannot be the case that Linda is a feminist bank teller without also being a bank teller. In an intensional reasoning scenario the goal is to identify the meaning of the ideas being described or communicated. Intensional reasoning allows a conjunction to be more likely than a constituent: if my intent is to communicate “red circle” to you, and you infer “circle”, a communication failure has occurred. In an effective communicative system, it is necessary to be able to specify (and to infer) the smaller of two nested sets, and conjunction 'fallacies’ are necessarily permitted. Consequently, while probabilistic reasoning models based on extensional logic do not produce conjunction fallacies, it is entirely possible for an intensional reasoning system to do so.\\Motivated by this theoretical perspective we present a series of experiments showing that people's behaviour in these tasks is highly sensitive to the distinction between extensional and intensional semantics. When a reasoning problem is framed in a way that emphasises the communicative and social aspect to the situation, strong conjunction effects appear. When the task is reframed to emphasise the extensional and non-social aspects, the fallacy is either attenuated or absent. This sensitivity occurs across many different social categories (e.g. feminist bank tellers) as well as reasoning about purely physical events (dice rolls). We argue that this sensitivity to framing occurs because people switch between solving different inference problems, both of which are sensible but are not equivalent to each other.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This project uses Bayesian Linear Ballistic Accumulator (LBA) models of decision-making to model the cognitive control mechanisms that aid prospective memory (PM) and ongoing task performance in a complex and dynamic air-traffic control (ATC) simulation. We aim to explain how operators balance competing demands from ongoing and PM tasks under different levels of time pressure, task load, and relative response importance.\\The ATC task involved classifying pairs of moving aircraft as either 'in-conflict' or 'not in-conflict'. On some trials aircraft also contained a PM target which required execution of an atypical PM response. These decisions require the integration of multiple information sources (e.g., relative distance, airspeed) on a dynamic display while balancing several competing task requirements (e.g., time pressure, PM demands, relative response importance). Moreover, decisions typically unfolded over relatively long time-scales (up to 10 seconds). Initial work suggests that models of simple choice such as the LBA can account for ongoing and PM task performance in these complex, long time-scale, less controlled applied settings.\\Our modelling shows evidence of both proactive and reactive control mechanisms. In terms of proactive control, response thresholds were higher under PM load. This suggests individuals proactively raise ongoing task thresholds when holding PM intentions. This effect was larger when the importance of the PM task was emphasised and smaller when the importance of the ongoing task was emphasised. This suggests that holding PM intentions encourages operators to make deliberate strategic adjustments to how they perform their primary ongoing task, and that these adjustments vary systematically as a function of PM task importance. </t>
+  </si>
+  <si>
+    <t>A popular way to estimate how words are similar involves asking participants to assign a magnitude judgement of similarity for a pair of words using a rating scale. This method has various limitations associated with the use of rating scales and lack of context when only two items are compared. Moreover, from a practical point of view, the procedure becomes prohibitively expensive for a large number of items. For example, for 1,000 items, obtaining one observation per pair would require nearly half a million judgements.\\In two studies, we explore an alternative procedure in which  participants either generate or rank a small number of near neighbours to a natural language concept. To evaluate the validity of this new task, we used pair-wise similarities collected for 15 basic level categories such as “birds” or “tools”. For each of the categories, we construct a sparse near neighbour graph and show that a mechanism of spreading activation based on random walks (see De Deyne, Navarro, Perfors &amp; Storms, 2016) can be used to accurately predict pair-wise similarity judgements using a limited amount of information.\\While these results suggest excellent external validity at a fraction of the cost, we also discuss some theoretical implications about the number of near neighbours and fundamental differences between similarity-based and feature-based inference in natural language concepts.</t>
+  </si>
+  <si>
+    <t>We present a model that predicts when people will believe events from their lives occurred on a person by person and stimulus by stimulus basis. Participants wore a smartphone in a pouch around their necks for two weeks. The smartphone collected timestamps, GPS, accelerometry, audio segments and images. These data sources were augmented with weather conditions, temperature, moon phase and tags derived from the audio using a machine learning model. A week later they were shown a selection of images and were required to indicate on which day each was taken. A conditional logit model predicted leave one person out judgements, leave one day out judgements and leave one observation out judgements. We highlight the advantages of using cross validation over other methods of model selection.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decisions from experience often differ from decisions based on described alternatives. This may stem from the fact that decisions from experience require that individuals learn about their choice alternatives by observing potential outcomes. We investigated the roles of attention and memory in the choice process by comparing two types of decision procedures: a) one where monetary value information is present during sampling, and b) one where values are revealed after sampling. In three experiments participants made a series of choices between pairs of risky gambles represented as urns containing different mixtures of blue and red balls. They began each trial by sampling balls from each urn. After observing a representative sample from each urn, participants chose which urn they would like to draw from for a consequential payment. In Experiment 3 some outcome samples were highlighted to increase visual and auditory salience.\\Results from all three experiments suggest that individuals place greater weight on rare events when outcome values are absent during sampling. This pattern is roughly consistent with the ‘description-experience gap’, in which decisions from description – which likewise involve separable representations of value and probability information – also indicate greater weighting of rare events relative to decisions from experience – which do not. In Experiment 3, we found that highlighting a rare reward increased its salience when outcome values were present, but not when they were absent, suggesting that highlighting rare outcome values during sampling led participants to place greater weight on these outcomes when making their choices. Parameter estimates from a hierarchical Bayesian prospect theory model supported the conclusion that value-absent choices involved greater overweighting of rare events. We discuss the implications of these findings on our understanding of the interplay between attention, memory, and choice. </t>
+  </si>
+  <si>
+    <t>What forensic experts should say, or should be allowed to say, about the results of forensic comparisons has been a contentious issue in the legal and forensic science communities. It is common practice for forensic pattern identification experts, such as in fingerprints and ballistics, to testify that two impressions originate from the same source to the exclusion of all others in the absence of statistical information. Experts have even claimed 100% accuracy, or that the rates of error are so improbable that they need not be considered. An alternative framework is necessary. When, if ever, should experts claim to have determined that two items share a common source, and should they present error rates, or the probability of coincidental matches?\\Here we explore options for the statistical representation and communication of forensic evidence in court. We argue that we have reached a turning point, where Australian state and federal police jurisdictions are seeking alternative frameworks for presenting evidence in court, but where well-considered proposals are scarce. We propose an avenue by which the mathematical psychology community might lend their own expertise to the problem.</t>
+  </si>
+  <si>
+    <t>Throughout the last few decades, a heated debate has been going on between frequentists and Bayesians. There are substantial theoretical and philosophical differences between both methods. Recently, a number of papers have come out claiming that for pragmatic purposes, both philosophies may not be all that different. In this presentation, I will discuss work that examines numerical correspondence between frequentist confidence intervals and Bayesian credible intervals based on non-informative priors. I show that numerically the differences between confidence intervals and credible intervals are very often negligible. I'll conclude with my take on the consequences of this for the frequentist-Bayesian debate from a practical viewpoint.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source memory is memory for the context in which items were previously encountered. Past research has largely aimed to establish whether source memory retrieval is better characterised as a threshold or continuous process in two-alternative forced choice tasks, using ROC functions. Recently, Harlow and Donaldson (2013) introduced a continuous report paradigm to study performance in source memory tasks, and found evidence of a retrieval threshold underlying response accuracy. However, this account does not consider response time (RT) distributions. To investigate the role of decision-making in source memory retrieval, this study used the Smith (2016) circular diffusion model to introduce diffusion analogues of the threshold and continuous models of source memory retrieval in a replication of the Harlow and Donaldson (2013) task. Model selection done using the BIC found support for a circular diffusion model where memory discretely fails, as both RT and response accuracy data suggested that there were two components in performance. </t>
+  </si>
+  <si>
+    <t>**MODELLING SPEEDED MULTIELEMENT DECISION MAKING AS DIFFUSION IN A HYPERSPHERE**</t>
+  </si>
+  <si>
+    <t>**ALTERNATIVE STATISTICAL FRAMEWORKS FOR COMMUNICATING THE STRENGTH OF FORENSIC EVIDENCE IN COURT**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In the real world we are often faced with decisions in which the possible outcomes are extremely good or bad but the probability of that outcome is extremely low: winning the lottery or being struck by lightning are prototypical examples. Should you buy a lottery ticket? Should you climb to the top of a hill in a rainstorm? These kind of situations are known colloquially as 'Black Swan'; scenarios and create a particularly hard decision problem. However, despite decades of research, decision theory is relatively silent about how people do (or should) reason about them: most of the standard tasks involve probabilities ranging between 10% to 90% and the outcomes are a manageable fraction of existing savings. In this study we evaluate how people reason in situations when one or both options involve extremely low probabilities (from 0.1 to 1.5%) of very bad outcomes (losing all of the points accumulated so far). We explore how decisions change as a function of the number of points available and the number of 'black swan'; options available. In addition, we evaluate if people's approach varies based on whether they are making a single bet or planning a strategy of bets over multiple games. Finally, we present some exploratory research investigating whether individual differences in anxiety and tolerance of uncertainty predict differences in behaviour in black swan situations. </t>
+  </si>
+  <si>
+    <t>We generalize the circular 2D diffusion model of Smith (2016) to provide a new model of speeded decision-making in multielement visual displays. We model decision making in tasks with multielement displays as evidence accumulation by a vector-valued diffusion process in a hypersphere, whose radius represents the decision criterion for the task. We show that the methods used to derive response time and accuracy predictions for the 2D model can be applied, with only minor changes, to predict performance in higher dimensional spaces as well. We apply the model to the double-target deficit paradigm of Duncan (1980) in which participants judge whether briefly-presented four-element displays contain one or two digit targets among letter distractors. A 4D version of the hyperspherical diffusion model correctly predicted distributions of response times and response accuracy as a function of task difficulty in single-target and double-target versions of the task. The estimated drift rate parameters from the model imply that the mental representation of the decision alternatives, which we term the 'decision template' for the task, encodes both configural and local stimulus properties. Along with its application to multielement decision making, the model has the potential to characterize the speed and accuracy of multiattribute decisions in studies of cognitive categorization, visual attention, and other areas.</t>
+  </si>
+  <si>
+    <t>I present a model for decision making for stimuli and responses in continuous space.  The model is applied to three numeracy tasks: in one, a two-digit number is presented and the participant has to move their finger to a matching location on a number line, in the second, an array of dots is presented and the participant is to move their finger to a matching location on an arc, and in the third, an array of dots is presented and the participant has to speak the number.  The model is composed of diffusion processes on lines and planes in which evidence from a stimulus (distributed across space) drives the noisy decision process which accumulates evidence over time to a criterion at which point a response is initiated.  Noise is represented as a continuous Gaussian process. The model produces fits for the full distributions of response times and choice probabilities across the stimulus space and provides distributed stimulus acuity measures.</t>
+  </si>
+  <si>
+    <t>Risky choice involves selection between two or more options each of which is a set of *n* ordered pairs, ($p_i,x_i$) , where $x_i$ is a (positive, negative, or zero) payoff and $p_i$ is its probability of occurrence, with  (\sum_i^n p_i=1 \).  There are a large number of different models of risky choice that fall into two broad classes; fixed utility models that satisfy the condition of *simple scalability* and everything else. A prominent example of the former is Cumulative Prospect Theory (Tversky &amp; Kahneman, 1992); a prominent example of the latter is Decision Field Theory (Busemeyer &amp; Townsend, 1993). While it is known that behaviour can be observed that inconsistent with all models, this has largely been based on the construction of special cases. We decided to test the class of fixed utility models against a set of relatively unselected risky choices using signed difference analysis (SDA). The advantage of this approach is that there is no requirement to posit a particular form for the error function that links the difference in the utility of two gambles, *A* and *B*, with the probability of choosing *A* over *B*, $ P(A \succ B) $ . We presented groups of participants with 30 *variable* gambles (*A*) each paired with one of four *fixed* gambles (*B*) and tested the prediction of fixed utility models that $P(A \succ B)$ has the same order over *A* for all *B* using the statistical test developed by Kalish, Dunn, Burdakov and Sysoev (2016). We discuss the implications of the results and explore a relatively simple extension to a (minimally) more complex model.\\ \\*References* \\Busemeyer, J. R., &amp; Townsend, J. T. (1993) Decision Field Theory: A dynamic cognition approach to decision making. *Psychological Review, 100*, 432–459.\\ \\Kalish, M. L., Dunn, J. C., Burdakov, O. P., &amp; Sysoev, O. (2016). A statistical test for equality of latent orders. *Journal of Mathematical Psychology, 70*, 1-11\\ \\Tversky, A. &amp; Kahneman, D. (1992). Advances in prospect theory: Cumulative representation of uncertainty. *Journal of Risk and Uncertainty, 5(4)*, 297–323.</t>
   </si>
 </sst>
 </file>
@@ -2803,14 +2771,14 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="303">
@@ -3455,8 +3423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="94" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="47.1640625" defaultRowHeight="26" x14ac:dyDescent="0.3"/>
@@ -3483,59 +3451,59 @@
         <v>0</v>
       </c>
       <c r="E1" s="137" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A2" s="137" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B2" s="137" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="137" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="D2" s="137" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="E2" s="137" t="s">
-        <v>87</v>
+        <v>408</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="182" x14ac:dyDescent="0.3">
       <c r="A3" s="137" t="s">
-        <v>420</v>
+        <v>402</v>
       </c>
       <c r="B3" s="137" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C3" s="137" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="D3" s="137" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="E3" s="137" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="139"/>
-    </row>
-    <row r="4" spans="1:6" ht="312" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="F3" s="138"/>
+    </row>
+    <row r="4" spans="1:6" ht="286" x14ac:dyDescent="0.3">
       <c r="A4" s="137" t="s">
-        <v>418</v>
+        <v>400</v>
       </c>
       <c r="B4" s="137" t="s">
-        <v>421</v>
+        <v>403</v>
       </c>
       <c r="C4" s="137" t="s">
-        <v>331</v>
-      </c>
-      <c r="D4" s="139" t="s">
-        <v>422</v>
+        <v>320</v>
+      </c>
+      <c r="D4" s="138" t="s">
+        <v>404</v>
       </c>
       <c r="E4" s="137" t="s">
-        <v>90</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
@@ -3543,285 +3511,285 @@
         <v>10</v>
       </c>
       <c r="B5" s="137" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="C5" s="137" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="D5" s="137" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="E5" s="137" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="390" x14ac:dyDescent="0.3">
       <c r="A6" s="137" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B6" s="137" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="C6" s="137" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
       <c r="D6" s="137" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="E6" s="137" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7" s="137" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B7" s="137" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C7" s="137" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
       <c r="D7" s="137" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="E7" s="137" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="390" x14ac:dyDescent="0.3">
       <c r="A8" s="137" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B8" s="137" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="C8" s="137" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="D8" s="137" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="E8" s="137" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="390" x14ac:dyDescent="0.3">
       <c r="A9" s="137" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B9" s="137" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="C9" s="137" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="D9" s="137" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="E9" s="137" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="260" x14ac:dyDescent="0.3">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="234" x14ac:dyDescent="0.3">
       <c r="A10" s="137" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B10" s="137" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="C10" s="137" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="D10" s="137" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="E10" s="137" t="s">
-        <v>113</v>
+        <v>414</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="312" x14ac:dyDescent="0.3">
       <c r="A11" s="137" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B11" s="137" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C11" s="137" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="D11" s="137" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="E11" s="137" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="364" x14ac:dyDescent="0.3">
       <c r="A12" s="137" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B12" s="137" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
       <c r="C12" s="137" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="D12" s="137" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="E12" s="137" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A13" s="137" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="137" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="C13" s="137" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="D13" s="137" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="E13" s="137" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="390" x14ac:dyDescent="0.3">
       <c r="A14" s="137" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B14" s="137" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C14" s="137" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="D14" s="137" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="E14" s="137" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A15" s="137" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B15" s="137" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="C15" s="137" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="D15" s="137" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="E15" s="137" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A16" s="137" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="137" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="C16" s="137" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="D16" s="137" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="E16" s="137" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="260" x14ac:dyDescent="0.3">
       <c r="A17" s="137" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B17" s="137" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C17" s="137" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="D17" s="137" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="E17" s="137" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A18" s="137" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="137" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="C18" s="137" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
       <c r="D18" s="137" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="E18" s="137" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A19" s="137" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="137" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="C19" s="137" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="D19" s="137" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="E19" s="137" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="364" x14ac:dyDescent="0.3">
       <c r="A20" s="137" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="137" t="s">
+        <v>279</v>
+      </c>
+      <c r="C20" s="137" t="s">
+        <v>331</v>
+      </c>
+      <c r="D20" s="137" t="s">
+        <v>373</v>
+      </c>
+      <c r="E20" s="137" t="s">
         <v>81</v>
-      </c>
-      <c r="B20" s="137" t="s">
-        <v>290</v>
-      </c>
-      <c r="C20" s="137" t="s">
-        <v>342</v>
-      </c>
-      <c r="D20" s="137" t="s">
-        <v>385</v>
-      </c>
-      <c r="E20" s="137" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A21" s="137" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B21" s="137" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="C21" s="137" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="D21" s="137" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="E21" s="137" t="s">
         <v>415</v>
@@ -3829,427 +3797,427 @@
     </row>
     <row r="22" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A22" s="137" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="137" t="s">
+        <v>277</v>
+      </c>
+      <c r="C22" s="137" t="s">
+        <v>333</v>
+      </c>
+      <c r="D22" s="137" t="s">
+        <v>375</v>
+      </c>
+      <c r="E22" s="137" t="s">
         <v>22</v>
-      </c>
-      <c r="B22" s="137" t="s">
-        <v>288</v>
-      </c>
-      <c r="C22" s="137" t="s">
-        <v>344</v>
-      </c>
-      <c r="D22" s="137" t="s">
-        <v>387</v>
-      </c>
-      <c r="E22" s="137" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A23" s="137" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B23" s="137" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="C23" s="137" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="D23" s="137" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="E23" s="137" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="260" x14ac:dyDescent="0.3">
       <c r="A24" s="137" t="s">
-        <v>419</v>
+        <v>401</v>
       </c>
       <c r="B24" s="137" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C24" s="137" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="D24" s="137" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="E24" s="137" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="338" x14ac:dyDescent="0.3">
       <c r="A25" s="137" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B25" s="137" t="s">
-        <v>287</v>
-      </c>
-      <c r="C25" s="138" t="s">
-        <v>346</v>
+        <v>276</v>
+      </c>
+      <c r="C25" s="140" t="s">
+        <v>407</v>
       </c>
       <c r="D25" s="137" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="E25" s="137" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A26" s="137" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B26" s="137" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="C26" s="137" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="D26" s="137" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="E26" s="137" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="130" x14ac:dyDescent="0.3">
       <c r="A27" s="137" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B27" s="137" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="C27" s="137" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="D27" s="137" t="s">
-        <v>390</v>
-      </c>
-      <c r="E27" s="140" t="s">
-        <v>424</v>
+        <v>378</v>
+      </c>
+      <c r="E27" s="139" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="234" x14ac:dyDescent="0.3">
       <c r="A28" s="137" t="s">
-        <v>417</v>
+        <v>399</v>
       </c>
       <c r="B28" s="137" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C28" s="137" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
       <c r="D28" s="137" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="E28" s="137" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A29" s="137" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B29" s="137" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="C29" s="137" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="D29" s="137" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="E29" s="137" t="s">
-        <v>116</v>
+        <v>411</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="234" x14ac:dyDescent="0.3">
       <c r="A30" s="137" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="137" t="s">
-        <v>54</v>
-      </c>
       <c r="C30" s="137" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="D30" s="137" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="E30" s="137" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="338" x14ac:dyDescent="0.3">
       <c r="A31" s="137" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="137" t="s">
+        <v>270</v>
+      </c>
+      <c r="C31" s="137" t="s">
+        <v>340</v>
+      </c>
+      <c r="D31" s="137" t="s">
+        <v>382</v>
+      </c>
+      <c r="E31" s="137" t="s">
         <v>15</v>
-      </c>
-      <c r="B31" s="137" t="s">
-        <v>281</v>
-      </c>
-      <c r="C31" s="137" t="s">
-        <v>352</v>
-      </c>
-      <c r="D31" s="137" t="s">
-        <v>394</v>
-      </c>
-      <c r="E31" s="137" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="286" x14ac:dyDescent="0.3">
       <c r="A32" s="137" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="137" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="C32" s="137" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="D32" s="137" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="E32" s="137" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="390" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="364" x14ac:dyDescent="0.3">
       <c r="A33" s="137" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="137" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C33" s="137" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="D33" s="137" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="E33" s="137" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="260" x14ac:dyDescent="0.3">
       <c r="A34" s="137" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="B34" s="137" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="C34" s="137" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="D34" s="137" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="E34" s="137" t="s">
-        <v>152</v>
+        <v>423</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="338" x14ac:dyDescent="0.3">
       <c r="A35" s="137" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="137" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="C35" s="137" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="D35" s="137" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="E35" s="137" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="286" x14ac:dyDescent="0.3">
       <c r="A36" s="137" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" s="137" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="C36" s="137" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="D36" s="137" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="E36" s="137" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="390" x14ac:dyDescent="0.3">
       <c r="A37" s="137" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B37" s="137" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C37" s="137" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="D37" s="137" t="s">
-        <v>400</v>
+        <v>419</v>
       </c>
       <c r="E37" s="137" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A38" s="137" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B38" s="137" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="C38" s="137" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="D38" s="137" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="E38" s="137" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A39" s="137" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" s="137" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="C39" s="137" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="D39" s="137" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="E39" s="137" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="364" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="338" x14ac:dyDescent="0.3">
       <c r="A40" s="137" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B40" s="137" t="s">
-        <v>273</v>
+        <v>406</v>
       </c>
       <c r="C40" s="137" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="D40" s="137" t="s">
-        <v>404</v>
+        <v>420</v>
       </c>
       <c r="E40" s="137" t="s">
-        <v>110</v>
+        <v>416</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A41" s="137" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="137" t="s">
+        <v>262</v>
+      </c>
+      <c r="C41" s="137" t="s">
+        <v>350</v>
+      </c>
+      <c r="D41" s="137" t="s">
+        <v>391</v>
+      </c>
+      <c r="E41" s="137" t="s">
         <v>105</v>
       </c>
-      <c r="B41" s="137" t="s">
-        <v>272</v>
-      </c>
-      <c r="C41" s="137" t="s">
-        <v>362</v>
-      </c>
-      <c r="D41" s="137" t="s">
-        <v>405</v>
-      </c>
-      <c r="E41" s="137" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="260" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:5" ht="208" x14ac:dyDescent="0.3">
       <c r="A42" s="137" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B42" s="137" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="C42" s="137" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="D42" s="137" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="E42" s="137" t="s">
-        <v>145</v>
+        <v>417</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A43" s="137" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="B43" s="137" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="C43" s="137" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
       <c r="D43" s="137" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="E43" s="137" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="338" x14ac:dyDescent="0.3">
       <c r="A44" s="137" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B44" s="137" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C44" s="137" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="D44" s="137" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="E44" s="137" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A45" s="137" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B45" s="137" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C45" s="137" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
       <c r="D45" s="137" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="E45" s="137" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="364" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="286" x14ac:dyDescent="0.3">
       <c r="A46" s="137" t="s">
         <v>13</v>
       </c>
       <c r="B46" s="137" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="C46" s="137" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="D46" s="137" t="s">
-        <v>410</v>
+        <v>396</v>
       </c>
       <c r="E46" s="137" t="s">
-        <v>14</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>
@@ -4288,10 +4256,10 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>7</v>
@@ -4306,7 +4274,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
@@ -4335,11 +4303,11 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="3" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="49" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -4347,28 +4315,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="53" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C4" s="49" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D4" s="50" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E4" s="51" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F4" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="49" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="52" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -4376,25 +4344,25 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -4402,25 +4370,25 @@
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="35" customFormat="1" x14ac:dyDescent="0.2">
@@ -4428,25 +4396,25 @@
         <v>1</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F7" s="116" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G7" s="116" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="35" t="s">
         <v>5</v>
       </c>
       <c r="I7" s="62" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="101" customFormat="1" x14ac:dyDescent="0.2">
@@ -4455,10 +4423,10 @@
       </c>
       <c r="D8" s="102"/>
       <c r="G8" s="101" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I8" s="103" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.2">
@@ -4470,28 +4438,28 @@
         <v>2</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H10" s="12" t="s">
         <v>5</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -4499,25 +4467,25 @@
         <v>2</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>5</v>
       </c>
       <c r="I11" s="17" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="15" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -4525,25 +4493,25 @@
         <v>2</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H12" s="15" t="s">
         <v>5</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -4551,25 +4519,25 @@
         <v>2</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F13" s="116" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G13" s="116" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H13" s="18" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.2">
@@ -4577,25 +4545,25 @@
         <v>2</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="E14" s="63" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F14" s="119" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G14" s="119" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H14" s="63" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="120" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.2">
@@ -4603,10 +4571,10 @@
         <v>2</v>
       </c>
       <c r="G15" s="63" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I15" s="63" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="64" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -4615,22 +4583,22 @@
         <v>3</v>
       </c>
       <c r="B17" s="73" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C17" s="74" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="75" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E17" s="74" t="s">
         <v>4</v>
       </c>
       <c r="F17" s="72" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17" s="74" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H17" s="72" t="s">
         <v>5</v>
@@ -4644,25 +4612,25 @@
         <v>3</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D18" s="55" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="E18" s="54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H18" s="54" t="s">
         <v>5</v>
       </c>
       <c r="I18" s="56" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="54" customFormat="1" x14ac:dyDescent="0.2">
@@ -4670,25 +4638,25 @@
         <v>3</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D19" s="57" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E19" s="54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G19" s="54" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H19" s="54" t="s">
         <v>5</v>
       </c>
       <c r="I19" s="58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="68" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -4696,25 +4664,25 @@
         <v>3</v>
       </c>
       <c r="C20" s="68" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D20" s="69" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E20" s="70" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F20" s="68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G20" s="68" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H20" s="68" t="s">
         <v>5</v>
       </c>
       <c r="I20" s="71" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="104" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -4724,10 +4692,10 @@
       <c r="D21" s="105"/>
       <c r="E21" s="106"/>
       <c r="G21" s="104" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I21" s="107" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="59" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -4740,28 +4708,28 @@
         <v>4</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D23" s="77" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>5</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -4769,25 +4737,25 @@
         <v>4</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E24" s="15" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H24" s="15" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="15" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -4795,25 +4763,25 @@
         <v>4</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="E25" s="15" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F25" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>5</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.2">
@@ -4821,25 +4789,25 @@
         <v>4</v>
       </c>
       <c r="C26" s="78" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="E26" s="78" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F26" s="78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G26" s="78" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H26" s="78" t="s">
         <v>5</v>
       </c>
       <c r="I26" s="79" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.2">
@@ -4847,25 +4815,25 @@
         <v>4</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D27" s="80" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F27" s="116" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G27" s="116" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I27" s="81" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="63" customFormat="1" x14ac:dyDescent="0.2">
@@ -4874,10 +4842,10 @@
       </c>
       <c r="D28" s="82"/>
       <c r="G28" s="63" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I28" s="83" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="64" customFormat="1" x14ac:dyDescent="0.2">
@@ -4889,28 +4857,28 @@
         <v>5</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D30" s="32" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H30" s="30" t="s">
         <v>5</v>
       </c>
       <c r="I30" s="33" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
@@ -4918,25 +4886,25 @@
         <v>5</v>
       </c>
       <c r="C31" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="E31" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="27" t="s">
-        <v>201</v>
-      </c>
-      <c r="E31" s="22" t="s">
-        <v>62</v>
-      </c>
       <c r="F31" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G31" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H31" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I31" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
@@ -4944,25 +4912,25 @@
         <v>5</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D32" s="25" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I32" s="26" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
@@ -4971,25 +4939,25 @@
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="E33" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="D33" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="E33" s="22" t="s">
+      <c r="F33" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H33" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="I33" s="24" t="s">
         <v>66</v>
-      </c>
-      <c r="F33" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="G33" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="I33" s="24" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
@@ -4998,25 +4966,25 @@
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E34" s="22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I34" s="41" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="89" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -5024,28 +4992,28 @@
         <v>5</v>
       </c>
       <c r="B35" s="89" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C35" s="89" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D35" s="90" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="E35" s="91" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F35" s="89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G35" s="89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H35" s="89" t="s">
         <v>5</v>
       </c>
       <c r="I35" s="92" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="108" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -5055,10 +5023,10 @@
       <c r="D36" s="109"/>
       <c r="E36" s="110"/>
       <c r="G36" s="108" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I36" s="111" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="59" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -5071,28 +5039,28 @@
         <v>6</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G38" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H38" s="12" t="s">
         <v>5</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="15" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -5100,25 +5068,25 @@
         <v>6</v>
       </c>
       <c r="C39" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E39" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>39</v>
-      </c>
       <c r="F39" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H39" s="15" t="s">
         <v>5</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="15" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -5126,25 +5094,25 @@
         <v>6</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E40" s="29" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F40" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G40" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H40" s="15" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I40" s="20" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="18" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -5152,25 +5120,25 @@
         <v>6</v>
       </c>
       <c r="C41" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="E41" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="37" t="s">
-        <v>208</v>
-      </c>
-      <c r="E41" s="18" t="s">
+      <c r="F41" s="116" t="s">
+        <v>51</v>
+      </c>
+      <c r="G41" s="116" t="s">
+        <v>74</v>
+      </c>
+      <c r="H41" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="I41" s="38" t="s">
         <v>50</v>
-      </c>
-      <c r="F41" s="116" t="s">
-        <v>52</v>
-      </c>
-      <c r="G41" s="116" t="s">
-        <v>75</v>
-      </c>
-      <c r="H41" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="I41" s="38" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="63" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -5179,10 +5147,10 @@
       </c>
       <c r="D42" s="93"/>
       <c r="G42" s="63" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I42" s="94" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="64" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -5194,28 +5162,28 @@
         <v>7</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C44" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="44" t="s">
+        <v>200</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="F44" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="I44" s="45" t="s">
         <v>73</v>
-      </c>
-      <c r="D44" s="44" t="s">
-        <v>209</v>
-      </c>
-      <c r="E44" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="F44" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="G44" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H44" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="I44" s="45" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.2">
@@ -5223,25 +5191,25 @@
         <v>7</v>
       </c>
       <c r="C45" s="39" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D45" s="42" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E45" s="39" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F45" s="39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G45" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H45" s="39" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I45" s="41" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
@@ -5249,25 +5217,25 @@
         <v>7</v>
       </c>
       <c r="C46" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="H46" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="I46" s="24" t="s">
         <v>19</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>211</v>
-      </c>
-      <c r="E46" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="F46" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="G46" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="H46" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="I46" s="24" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="22" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -5275,25 +5243,25 @@
         <v>7</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H47" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
@@ -5304,22 +5272,22 @@
         <v>13</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E48" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F48" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G48" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H48" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I48" s="26" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="89" customFormat="1" ht="19" x14ac:dyDescent="0.2">
@@ -5327,25 +5295,25 @@
         <v>7</v>
       </c>
       <c r="C49" s="89" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D49" s="99" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E49" s="89" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F49" s="89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G49" s="89" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H49" s="89" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I49" s="100" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="108" customFormat="1" x14ac:dyDescent="0.2">
@@ -5354,10 +5322,10 @@
       </c>
       <c r="D50" s="112"/>
       <c r="G50" s="108" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I50" s="113" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:9" s="59" customFormat="1" x14ac:dyDescent="0.2">
@@ -5369,28 +5337,28 @@
         <v>8</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C52" s="30" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="E52" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D52" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="E52" s="30" t="s">
+      <c r="F52" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G52" s="30" t="s">
+        <v>84</v>
+      </c>
+      <c r="H52" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="I52" s="45" t="s">
         <v>59</v>
-      </c>
-      <c r="F52" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="G52" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="H52" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="I52" s="45" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:9" s="22" customFormat="1" x14ac:dyDescent="0.2">
@@ -5401,19 +5369,19 @@
         <v>10</v>
       </c>
       <c r="D53" s="25" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E53" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G53" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H53" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I53" s="24" t="s">
         <v>12</v>
@@ -5424,25 +5392,25 @@
         <v>8</v>
       </c>
       <c r="C54" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="D54" s="27" t="s">
         <v>53</v>
       </c>
-      <c r="D54" s="27" t="s">
+      <c r="E54" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="E54" s="22" t="s">
-        <v>55</v>
-      </c>
       <c r="F54" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G54" s="22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H54" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I54" s="34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -5451,25 +5419,25 @@
       </c>
       <c r="B55" s="22"/>
       <c r="C55" s="39" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D55" s="40" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="E55" s="39" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F55" s="39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G55" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H55" s="39" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I55" s="43" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
@@ -5478,25 +5446,25 @@
       </c>
       <c r="B56" s="22"/>
       <c r="C56" s="39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E56" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="F56" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="D56" s="40" t="s">
-        <v>218</v>
-      </c>
-      <c r="E56" s="39" t="s">
+      <c r="G56" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="H56" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="I56" s="41" t="s">
         <v>86</v>
-      </c>
-      <c r="F56" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="G56" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="H56" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="I56" s="41" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.2">
@@ -5504,25 +5472,25 @@
         <v>8</v>
       </c>
       <c r="C57" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E57" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F57" s="118" t="s">
+        <v>51</v>
+      </c>
+      <c r="G57" s="118" t="s">
+        <v>84</v>
+      </c>
+      <c r="H57" s="39" t="s">
+        <v>146</v>
+      </c>
+      <c r="I57" s="41" t="s">
         <v>70</v>
-      </c>
-      <c r="D57" s="42" t="s">
-        <v>219</v>
-      </c>
-      <c r="E57" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="F57" s="118" t="s">
-        <v>52</v>
-      </c>
-      <c r="G57" s="118" t="s">
-        <v>85</v>
-      </c>
-      <c r="H57" s="39" t="s">
-        <v>155</v>
-      </c>
-      <c r="I57" s="41" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="114" customFormat="1" x14ac:dyDescent="0.2">
@@ -5530,22 +5498,22 @@
         <v>8</v>
       </c>
       <c r="C58" s="114" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D58" s="115" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="E58" s="114" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F58" s="114" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G58" s="114" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I58" s="114" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="1:9" s="22" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -5553,25 +5521,25 @@
         <v>8</v>
       </c>
       <c r="C59" s="47" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D59" s="48" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E59" s="48" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F59" s="117" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G59" s="117" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H59" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I59" s="48" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -5579,10 +5547,10 @@
         <v>8</v>
       </c>
       <c r="G60" s="39" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -5590,7 +5558,7 @@
         <v>8</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -5630,10 +5598,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="121" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="B1" s="121" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C1" s="121" t="s">
         <v>7</v>
@@ -5648,7 +5616,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="121" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H1" s="121" t="s">
         <v>2</v>
@@ -5657,7 +5625,7 @@
         <v>0</v>
       </c>
       <c r="J1" s="121" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -5665,10 +5633,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I3" s="123" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -5676,28 +5644,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="121" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C4" s="121" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="122" t="s">
+        <v>252</v>
+      </c>
+      <c r="E4" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="122" t="s">
-        <v>262</v>
-      </c>
-      <c r="E4" s="121" t="s">
-        <v>39</v>
-      </c>
       <c r="F4" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G4" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H4" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I4" s="123" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.25">
@@ -5705,25 +5673,25 @@
         <v>1</v>
       </c>
       <c r="C5" s="121" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="124" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="E5" s="121" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H5" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I5" s="123" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -5731,25 +5699,25 @@
         <v>1</v>
       </c>
       <c r="C6" s="121" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D6" s="124" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="E6" s="121" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F6" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6" s="121" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I6" s="125" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -5757,25 +5725,25 @@
         <v>1</v>
       </c>
       <c r="C7" s="121" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D7" s="124" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="E7" s="126" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F7" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H7" s="121" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I7" s="123" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -5783,25 +5751,25 @@
         <v>1</v>
       </c>
       <c r="C8" s="121" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="124" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" s="121" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="124" t="s">
-        <v>246</v>
-      </c>
-      <c r="E8" s="121" t="s">
+      <c r="F8" s="121" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="121" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="I8" s="125" t="s">
         <v>50</v>
-      </c>
-      <c r="F8" s="121" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="121" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="I8" s="125" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -5810,10 +5778,10 @@
       </c>
       <c r="D9" s="124"/>
       <c r="G9" s="121" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I9" s="125" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -5825,25 +5793,25 @@
         <v>2</v>
       </c>
       <c r="C11" s="121" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="122" t="s">
+        <v>245</v>
+      </c>
+      <c r="E11" s="121" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="121" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="121" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="I11" s="123" t="s">
         <v>70</v>
-      </c>
-      <c r="D11" s="122" t="s">
-        <v>255</v>
-      </c>
-      <c r="E11" s="121" t="s">
-        <v>69</v>
-      </c>
-      <c r="F11" s="121" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="121" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="I11" s="123" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="126" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -5851,25 +5819,25 @@
         <v>2</v>
       </c>
       <c r="C12" s="133" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="D12" s="136" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="E12" s="133" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="F12" s="133" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="133" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H12" s="126" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I12" s="135" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -5877,25 +5845,25 @@
         <v>2</v>
       </c>
       <c r="C13" s="121" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="124" t="s">
+        <v>243</v>
+      </c>
+      <c r="E13" s="121" t="s">
+        <v>85</v>
+      </c>
+      <c r="F13" s="121" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="124" t="s">
-        <v>253</v>
-      </c>
-      <c r="E13" s="121" t="s">
+      <c r="G13" s="121" t="s">
+        <v>84</v>
+      </c>
+      <c r="H13" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="I13" s="123" t="s">
         <v>86</v>
-      </c>
-      <c r="F13" s="121" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" s="121" t="s">
-        <v>85</v>
-      </c>
-      <c r="H13" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="I13" s="123" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -5903,25 +5871,25 @@
         <v>2</v>
       </c>
       <c r="C14" s="121" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="D14" s="122" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="E14" s="121" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="F14" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G14" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H14" s="121" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="I14" s="121" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -5929,25 +5897,25 @@
         <v>2</v>
       </c>
       <c r="C15" s="121" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D15" s="122" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="E15" s="121" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F15" s="121" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G15" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H15" s="121" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I15" s="123" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -5955,25 +5923,25 @@
         <v>2</v>
       </c>
       <c r="C16" s="121" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="124" t="s">
+        <v>238</v>
+      </c>
+      <c r="E16" s="121" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="121" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="121" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="121" t="s">
+        <v>146</v>
+      </c>
+      <c r="I16" s="123" t="s">
         <v>73</v>
-      </c>
-      <c r="D16" s="124" t="s">
-        <v>248</v>
-      </c>
-      <c r="E16" s="121" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="121" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="121" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="I16" s="123" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -5984,19 +5952,19 @@
         <v>10</v>
       </c>
       <c r="D17" s="124" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="E17" s="121" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F17" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H17" s="121" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I17" s="125" t="s">
         <v>12</v>
@@ -6011,10 +5979,10 @@
       <c r="E18" s="132"/>
       <c r="F18" s="126"/>
       <c r="G18" s="126" t="s">
+        <v>160</v>
+      </c>
+      <c r="I18" s="132" t="s">
         <v>169</v>
-      </c>
-      <c r="I18" s="132" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
@@ -6030,28 +5998,28 @@
         <v>3</v>
       </c>
       <c r="B20" s="121" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C20" s="121" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20" s="126" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="E20" s="121" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F20" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G20" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H20" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I20" s="123" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="38" x14ac:dyDescent="0.25">
@@ -6059,25 +6027,25 @@
         <v>3</v>
       </c>
       <c r="C21" s="121" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D21" s="126" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="E21" s="121" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="F21" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G21" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H21" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I21" s="123" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -6085,25 +6053,25 @@
         <v>3</v>
       </c>
       <c r="C22" s="121" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D22" s="121" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="E22" s="121" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F22" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G22" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H22" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I22" s="121" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -6111,25 +6079,25 @@
         <v>3</v>
       </c>
       <c r="C23" s="121" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D23" s="122" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="E23" s="121" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F23" s="121" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G23" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H23" s="121" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I23" s="127" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -6137,25 +6105,25 @@
         <v>3</v>
       </c>
       <c r="C24" s="121" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="D24" s="122" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E24" s="121" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F24" s="121" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G24" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H24" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I24" s="125" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -6163,10 +6131,10 @@
         <v>3</v>
       </c>
       <c r="G25" s="121" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="I25" s="127" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -6178,28 +6146,28 @@
         <v>4</v>
       </c>
       <c r="B27" s="121" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C27" s="121" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="D27" s="134" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="E27" s="133" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="F27" s="133" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G27" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H27" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I27" s="134" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -6207,25 +6175,25 @@
         <v>4</v>
       </c>
       <c r="C28" s="121" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D28" s="122" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E28" s="121" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F28" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G28" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H28" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I28" s="123" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -6233,25 +6201,25 @@
         <v>4</v>
       </c>
       <c r="C29" s="121" t="s">
+        <v>60</v>
+      </c>
+      <c r="D29" s="122" t="s">
+        <v>257</v>
+      </c>
+      <c r="E29" s="121" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="122" t="s">
-        <v>267</v>
-      </c>
-      <c r="E29" s="121" t="s">
-        <v>62</v>
-      </c>
       <c r="F29" s="121" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G29" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H29" s="121" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I29" s="123" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="22" x14ac:dyDescent="0.25">
@@ -6259,28 +6227,28 @@
         <v>4</v>
       </c>
       <c r="B30" s="121" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C30" s="121" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D30" s="126" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="E30" s="128" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="F30" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G30" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H30" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I30" s="127" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -6288,25 +6256,25 @@
         <v>4</v>
       </c>
       <c r="C31" s="121" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D31" s="124" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E31" s="121" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F31" s="121" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G31" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H31" s="121" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I31" s="123" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -6314,25 +6282,25 @@
         <v>4</v>
       </c>
       <c r="C32" s="121" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D32" s="124" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="E32" s="121" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F32" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G32" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H32" s="121" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I32" s="123" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -6341,10 +6309,10 @@
       </c>
       <c r="D33" s="124"/>
       <c r="G33" s="121" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="I33" s="125" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -6358,28 +6326,28 @@
         <v>5</v>
       </c>
       <c r="B36" s="121" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C36" s="121" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D36" s="124" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E36" s="126" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="F36" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G36" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H36" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I36" s="123" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -6387,25 +6355,25 @@
         <v>5</v>
       </c>
       <c r="C37" s="121" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D37" s="124" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="E37" s="121" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F37" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G37" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H37" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I37" s="125" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -6413,25 +6381,25 @@
         <v>5</v>
       </c>
       <c r="C38" s="121" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="D38" s="121" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="E38" s="121" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="F38" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G38" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H38" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I38" s="121" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -6439,25 +6407,25 @@
         <v>5</v>
       </c>
       <c r="C39" s="121" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D39" s="122" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="E39" s="121" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F39" s="121" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G39" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H39" s="121" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I39" s="125" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.25">
@@ -6465,25 +6433,25 @@
         <v>5</v>
       </c>
       <c r="C40" s="126" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="D40" s="132" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="E40" s="132" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="F40" s="126" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G40" s="126" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H40" s="121" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I40" s="132" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -6491,10 +6459,10 @@
         <v>5</v>
       </c>
       <c r="G41" s="121" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="I41" s="129" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -6505,28 +6473,28 @@
         <v>6</v>
       </c>
       <c r="B43" s="121" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C43" s="121" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D43" s="124" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E43" s="121" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F43" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G43" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H43" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I43" s="123" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -6534,25 +6502,25 @@
         <v>6</v>
       </c>
       <c r="C44" s="121" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D44" s="122" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="E44" s="121" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F44" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G44" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H44" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I44" s="123" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -6560,25 +6528,25 @@
         <v>6</v>
       </c>
       <c r="C45" s="121" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D45" s="121" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E45" s="121" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F45" s="121" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G45" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H45" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I45" s="121" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -6586,25 +6554,25 @@
         <v>6</v>
       </c>
       <c r="C46" s="121" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D46" s="121" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="E46" s="121" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F46" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G46" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H46" s="121" t="s">
         <v>11</v>
       </c>
       <c r="I46" s="125" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -6612,25 +6580,25 @@
         <v>6</v>
       </c>
       <c r="C47" s="121" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D47" s="122" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="E47" s="121" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F47" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G47" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H47" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I47" s="123" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -6638,25 +6606,25 @@
         <v>6</v>
       </c>
       <c r="C48" s="121" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="126" t="s">
+        <v>194</v>
+      </c>
+      <c r="E48" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="D48" s="126" t="s">
-        <v>203</v>
-      </c>
-      <c r="E48" s="121" t="s">
+      <c r="F48" s="121" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" s="121" t="s">
+        <v>84</v>
+      </c>
+      <c r="H48" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="I48" s="125" t="s">
         <v>66</v>
-      </c>
-      <c r="F48" s="121" t="s">
-        <v>75</v>
-      </c>
-      <c r="G48" s="121" t="s">
-        <v>85</v>
-      </c>
-      <c r="H48" s="121" t="s">
-        <v>154</v>
-      </c>
-      <c r="I48" s="125" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -6665,10 +6633,10 @@
       </c>
       <c r="D49" s="121"/>
       <c r="G49" s="121" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="I49" s="121" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -6680,22 +6648,22 @@
         <v>7</v>
       </c>
       <c r="B51" s="121" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C51" s="121" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="122" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E51" s="121" t="s">
         <v>4</v>
       </c>
       <c r="F51" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G51" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H51" s="121" t="s">
         <v>5</v>
@@ -6709,25 +6677,25 @@
         <v>7</v>
       </c>
       <c r="C52" s="121" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D52" s="122" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="E52" s="121" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F52" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G52" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H52" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I52" s="127" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -6735,25 +6703,25 @@
         <v>7</v>
       </c>
       <c r="C53" s="121" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D53" s="126" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="E53" s="121" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F53" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G53" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H53" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I53" s="125" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="22" x14ac:dyDescent="0.25">
@@ -6761,25 +6729,25 @@
         <v>7</v>
       </c>
       <c r="C54" s="121" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D54" s="122" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="E54" s="130" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="F54" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G54" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H54" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I54" s="125" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -6787,25 +6755,25 @@
         <v>7</v>
       </c>
       <c r="C55" s="121" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" s="122" t="s">
+        <v>241</v>
+      </c>
+      <c r="E55" s="121" t="s">
         <v>58</v>
       </c>
-      <c r="D55" s="122" t="s">
-        <v>251</v>
-      </c>
-      <c r="E55" s="121" t="s">
+      <c r="F55" s="121" t="s">
+        <v>74</v>
+      </c>
+      <c r="G55" s="121" t="s">
+        <v>84</v>
+      </c>
+      <c r="H55" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="I55" s="123" t="s">
         <v>59</v>
-      </c>
-      <c r="F55" s="121" t="s">
-        <v>75</v>
-      </c>
-      <c r="G55" s="121" t="s">
-        <v>85</v>
-      </c>
-      <c r="H55" s="121" t="s">
-        <v>154</v>
-      </c>
-      <c r="I55" s="123" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="22" x14ac:dyDescent="0.25">
@@ -6814,10 +6782,10 @@
       </c>
       <c r="E56" s="130"/>
       <c r="G56" s="121" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="I56" s="125" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="22" x14ac:dyDescent="0.25">
@@ -6829,25 +6797,25 @@
         <v>8</v>
       </c>
       <c r="C58" s="121" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D58" s="122" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="E58" s="121" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F58" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G58" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H58" s="121" t="s">
         <v>5</v>
       </c>
       <c r="I58" s="123" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -6855,25 +6823,25 @@
         <v>8</v>
       </c>
       <c r="C59" s="121" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="122" t="s">
+        <v>202</v>
+      </c>
+      <c r="E59" s="121" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59" s="121" t="s">
+        <v>51</v>
+      </c>
+      <c r="G59" s="121" t="s">
+        <v>84</v>
+      </c>
+      <c r="H59" s="121" t="s">
+        <v>145</v>
+      </c>
+      <c r="I59" s="125" t="s">
         <v>19</v>
-      </c>
-      <c r="D59" s="122" t="s">
-        <v>211</v>
-      </c>
-      <c r="E59" s="121" t="s">
-        <v>39</v>
-      </c>
-      <c r="F59" s="121" t="s">
-        <v>52</v>
-      </c>
-      <c r="G59" s="121" t="s">
-        <v>85</v>
-      </c>
-      <c r="H59" s="121" t="s">
-        <v>154</v>
-      </c>
-      <c r="I59" s="125" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -6881,19 +6849,19 @@
         <v>8</v>
       </c>
       <c r="C60" s="121" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D60" s="131" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="E60" s="121" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="G60" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I60" s="131" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
@@ -6901,25 +6869,25 @@
         <v>8</v>
       </c>
       <c r="C61" s="121" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D61" s="124" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="E61" s="121" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F61" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G61" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H61" s="121" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I61" s="125" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="22" x14ac:dyDescent="0.25">
@@ -6927,25 +6895,25 @@
         <v>8</v>
       </c>
       <c r="C62" s="121" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D62" s="122" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="E62" s="121" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F62" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G62" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H62" s="121" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I62" s="125" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -6956,22 +6924,22 @@
         <v>13</v>
       </c>
       <c r="D63" s="122" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="E63" s="121" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F63" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G63" s="121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H63" s="121" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I63" s="123" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="22" x14ac:dyDescent="0.25">
@@ -6980,10 +6948,10 @@
       </c>
       <c r="E64" s="130"/>
       <c r="G64" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I64" s="123" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="22" x14ac:dyDescent="0.25">
@@ -6993,7 +6961,7 @@
       <c r="D65" s="126"/>
       <c r="E65" s="128"/>
       <c r="I65" s="123" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="22" x14ac:dyDescent="0.25">

</xml_diff>